<commit_message>
Add Random forest alrotithm
</commit_message>
<xml_diff>
--- a/predicted.xlsx
+++ b/predicted.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.1</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.41</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.07</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.03</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.83</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.63</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.42</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.08</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.02</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2.84</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.99</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.88</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3.28</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3.83</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3.65</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>3.71</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3.58</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6.81</v>
+        <v>7.01</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3.77</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3.63</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3.87</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1.99</v>
+        <v>3.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Random forest algorithm
</commit_message>
<xml_diff>
--- a/predicted.xlsx
+++ b/predicted.xlsx
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>3.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">

</xml_diff>

<commit_message>
Tune Random forest algorithm
</commit_message>
<xml_diff>
--- a/predicted.xlsx
+++ b/predicted.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.13</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.36</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.22</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.32</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.33</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.2</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.07</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.3</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.2</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.2</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.08</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.08</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.21</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.24</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.12</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3.05</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.34</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2.34</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2.3</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2.36</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>7.01</v>
+        <v>6.87</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3.62</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3.75</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2.7</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="30">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>8.51</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2.53</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2.57</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3.04</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3.67</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="36">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3.43</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3.44</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3.49</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3.48</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2.61</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3.44</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="45">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>3.45</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3.44</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2.53</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2.56</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2.57</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.63</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2.62</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3.23</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>3.25</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>3.24</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="72">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>3.29</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>3.47</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>3.45</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>3.27</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>3.31</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3.28</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>3.27</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>3.24</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="83">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3.11</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>3.11</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>3.35</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>3.32</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>3.29</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>3.23</v>
+        <v>3.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing gradient boosting algorithms
</commit_message>
<xml_diff>
--- a/predicted.xlsx
+++ b/predicted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.11</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.31</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.23</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.24</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.2</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.27</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.19</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.04</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.23</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.14</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.15</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.1</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.16</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.13</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.08</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3.04</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="19">
@@ -628,131 +628,131 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BaTaO2N</t>
+          <t>Bi1.5Cr0.5Ti2O7</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.92</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BaTa0.5Al0.5O2N</t>
+          <t>Bi1.5Fe0.5Ti2O7</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BaTa0.5Mg0.5O2N</t>
+          <t>Bi4Ti2O11</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2.27</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BaTa0.5Al0.25Mg0.25O2N</t>
+          <t>Bi1.5Li0.5Ti2O7</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2.28</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BaTa0.5Al0.125Mg0.375O2N</t>
+          <t>Bi1.5Na0.5Ti2O7</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2.25</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BaTa0.5Al0.375Mg0.125O2N</t>
+          <t>Bi1.5Cu0.5Ti2O7</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Al2O3</t>
+          <t>Bi1.5Ag0.5Ti2O7</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6.87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TiO2</t>
+          <t>Bi1.5Mg0.5Ti2O7</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ta2O5</t>
+          <t>Bi1.5Ca0.5Ti2O7</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3.78</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Fe2O3</t>
+          <t>Bi1.5Zn0.5Ti2O7</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2.62</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NaLaTi2O6</t>
+          <t>Bi1.5Cd0.5Ti2O7</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3.6</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NaCl</t>
+          <t>Bi1.5Cr0.5Ti2O7</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>8.5</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bi1.5Cr0.5Ti2O7</t>
+          <t>Bi1.5Mn0.5Ti2O7</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -762,577 +762,937 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Bi4Ti2O11</t>
+          <t>Bi1.5Co0.5Ti2O7</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ta1.94Eu0.06O5</t>
+          <t>Bi1.5Ni0.5Ti2O7</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Bi1.5Li0.2Na0.2Mg0.5Nb1.5O6.7</t>
+          <t>Bi1.5Ce0.5Ti2O7</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bi1.3Li0.2Na0.2La0.2Mg0.5Nb1.5O6.7</t>
+          <t>Bi1.5Pr0.5Ti2O7</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>3.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Bi1.3Li0.2Na0.2Eu0.2Mg0.5Nb1.5O6.7</t>
+          <t>Bi1.5Nd0.5Ti2O7</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bi1.1Li0.2Na0.2Eu0.2Mg0.5Nb1.5O6.7</t>
+          <t>Bi1.5Pm0.5Ti2O7</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Bi1.5Li0.5Ti2O7</t>
+          <t>Bi1.5Sm0.5Ti2O7</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bi1.5Na0.5Ti2O7</t>
+          <t>Bi1.5Eu0.5Ti2O7</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bi1.5Cu0.5Ti2O7</t>
+          <t>Bi1.5Gd0.5Ti2O7</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bi1.5Ag0.5Ti2O7</t>
+          <t>Bi1.5Tb0.5Ti2O7</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bi1.5Mg0.5Ti2O7</t>
+          <t>Bi1.5Dy0.5Ti2O7</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3.39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bi1.5Ca0.5Ti2O7</t>
+          <t>Bi1.5Ho0.5Ti2O7</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3.39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bi1.5Zn0.5Ti2O7</t>
+          <t>Bi1.5Er0.5Ti2O7</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>3.37</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Bi1.5Cd0.5Ti2O7</t>
+          <t>Bi1.5Tm0.5Ti2O7</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Bi1.5Cr0.5Ti2O7</t>
+          <t>Bi1.5Yb0.5Ti2O7</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Bi1.5Mn0.5Ti2O7</t>
+          <t>Bi1.5Lu0.5Ti2O7</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2.62</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Bi1.5Fe0.5Ti2O7</t>
+          <t>Bi1.5Eu0.5Ti2O7</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Bi1.5Co0.5Ti2O7</t>
+          <t>Bi1.75Eu0.25Ti2O7</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Bi1.5Ni0.5Ti2O7</t>
+          <t>Bi1.875Eu0.125Ti2O7</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Bi1.5Ce0.5Ti2O7</t>
+          <t>Bi1.5Ho0.5Ti2O7</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Bi1.5Pr0.5Ti2O7</t>
+          <t>Bi1.75Ho0.25Ti2O7</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3.17</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Bi1.5Nd0.5Ti2O7</t>
+          <t>Bi1.875Ho0.125Ti2O7</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>3.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Bi1.5Pm0.5Ti2O7</t>
+          <t>Bi1.5Yb0.5Ti2O7</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Bi1.5Sm0.5Ti2O7</t>
+          <t>Bi1.75Yb0.25Ti2O7</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>3.2</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Bi1.5Eu0.5Ti2O7</t>
+          <t>Bi1.875Yb0.125Ti2O7</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Bi1.5Gd0.5Ti2O7</t>
+          <t>Bi1.6Li0.4Ti2O6.6</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3.21</v>
+        <v>3.84</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Bi1.5Tb0.5Ti2O7</t>
+          <t>Bi1.5Na0.125Ti2O6.3125</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>3.2</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Bi1.5Dy0.5Ti2O7</t>
+          <t>Bi1.5Ga0.25Ti2O6.625</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>3.2</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Bi1.5Ho0.5Ti2O7</t>
+          <t>Bi1.5In0.25Ti2O6.625</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>3.2</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Bi1.5Er0.5Ti2O7</t>
+          <t>Bi1.75In0.25Ti2O7</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3.21</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Bi1.5Tm0.5Ti2O7</t>
+          <t>Bi1.875In0.125Ti2O7</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>3.21</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Bi1.5Yb0.5Ti2O7</t>
+          <t>Bi1.9375In0.0625Ti2O7</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>3.3</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Bi1.5Lu0.5Ti2O7</t>
+          <t>Bi1.5Sc0.25Ti2O6.625</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3.22</v>
+        <v>3.63</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Bi1.5Eu0.5Ti2O7</t>
+          <t>Bi1.75Sc0.25Ti2O7</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>3.23</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Bi1.75Eu0.25Ti2O7</t>
+          <t>Bi1.875Sc0.125Ti2O7</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>3.19</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Bi1.875Eu0.125Ti2O7</t>
+          <t>Bi1.9375Sc0.0625Ti2O7</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>3.2</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Bi1.5Ho0.5Ti2O7</t>
+          <t>Bi1.5Al0.25Ti2O6.625</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3.2</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Bi1.75Ho0.25Ti2O7</t>
+          <t>Bi1.75Al0.25Ti2O7</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3.17</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Bi1.875Ho0.125Ti2O7</t>
+          <t>Bi1.875Al0.125Ti2O7</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>3.17</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Bi1.5Yb0.5Ti2O7</t>
+          <t>Bi1.9375Al0.0625Ti2O7</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>3.3</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Bi1.75Yb0.25Ti2O7</t>
+          <t>Ta1.94Eu0.06O5</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>3.27</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Bi1.875Yb0.125Ti2O7</t>
+          <t>BaTaO2N</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>3.25</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Bi1.6Li0.4Ti2O6.6</t>
+          <t>BaTa0.5Al0.5O2N</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>3.45</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Bi1.5Na0.125Ti2O6.3125</t>
+          <t>BaTa0.5Mg0.5O2N</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>3.41</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Bi1.5Ga0.25Ti2O6.625</t>
+          <t>BaTa0.5Al0.25Mg0.25O2N</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>3.22</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Bi1.5In0.25Ti2O6.625</t>
+          <t>BaTa0.5Al0.125Mg0.375O2N</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>3.27</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Bi1.75In0.25Ti2O7</t>
+          <t>BaTa0.5Al0.375Mg0.125O2N</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3.23</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Bi1.875In0.125Ti2O7</t>
+          <t>Al2O3</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>3.22</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Bi1.9375In0.0625Ti2O7</t>
+          <t>TiO2</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>3.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Bi1.5Sc0.25Ti2O6.625</t>
+          <t>Ta2O5</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>3.21</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Bi1.75Sc0.25Ti2O7</t>
+          <t>Fe2O3</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>3.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Bi1.875Sc0.125Ti2O7</t>
+          <t>NaLaTi2O6</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3.12</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Bi1.9375Sc0.0625Ti2O7</t>
+          <t>NaCl</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>3.12</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Bi1.5Al0.25Ti2O6.625</t>
+          <t>Bi1.5Mg1.0Nb1.5O7.0</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>3.31</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Bi1.75Al0.25Ti2O7</t>
+          <t>Bi1.5Mg0.9Na0.1Nb1.5O6.95</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>3.27</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Bi1.875Al0.125Ti2O7</t>
+          <t>Bi1.5Mg0.75Na0.25Nb1.5O6.875</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>3.22</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Bi1.9375Al0.0625Ti2O7</t>
+          <t>Bi1.5Mg0.65Na0.25Nb1.5O6.775</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>3.19</v>
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.5Na0.4Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.65Li0.25Nb1.5O6.775</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.5Li0.4Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Bi1.0Eu0.5Li0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Bi1.1Eu0.4Li0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Bi1.2Eu0.3Li0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Bi1.3Eu0.2Li0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Bi1.4Eu0.1Li0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Bi1.0Eu0.5Na0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Bi1.1Eu0.4Na0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Bi1.2Eu0.3Na0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Bi1.3Eu0.2Na0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Bi1.4Eu0.1Na0.4Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.9Nb1.5O6.9</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.5Al0.4Nb1.5O7.1</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Bi1.5Zn0.9Nb1.5O6.9</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Bi1.5Zn0.5Al0.4Nb1.5O7.1</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Bi1.3Li0.45Al0.45Nb1.5O6.6</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Bi1.3Li0.45Ga0.45Nb1.5O6.6</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Bi1.3Li0.45In0.45Nb1.5O6.6</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.5Ga0.4Nb1.5O7.1</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Bi1.5Mg0.5In0.4Nb1.5O7.1</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Bi1.5Zn0.5Ga0.4Nb1.5O7.1</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Bi1.5Zn0.5In0.4Nb1.5O7.1</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Bi1.3Na0.45Al0.45Nb1.5O6.6</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Bi1.3Na0.45Ga0.45Nb1.5O6.6</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Bi1.3Na0.45In0.45Nb1.5O6.6</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Bi1.56Cu0.19Mg0.58Nb1.56O7.01</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Bi1.56Cu0.39Mg0.39Nb1.56O7.02</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Bi1.46Li0.1Cu0.38Mg0.39Nb1.56O6.91</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Bi1.35Li0.21Cu0.38Mg0.39Nb1.56O6.8</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Bi1.5Li0.2Na0.2Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Bi1.3Li0.2Na0.2La0.2Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Bi1.3Li0.2Na0.2Eu0.2Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Bi1.1Li0.2Na0.2La0.2Eu0.2Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Bi0.9Li0.2Na0.2La0.3Eu0.3Mg0.5Nb1.5O6.7</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>